<commit_message>
Updated data model so that there is now 'data_type' in all data files (for Gen3 data validation purposes). Now also includes validated synthetic data.
</commit_message>
<xml_diff>
--- a/output/input_google_sheets/xlsx/prop_def.xlsx
+++ b/output/input_google_sheets/xlsx/prop_def.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="properties" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">properties!$A$1:$T$1002</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">properties!$A$1:$T$1005</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="111">
   <si>
     <t>VARIABLE_NAME</t>
   </si>
@@ -316,6 +316,12 @@
     <t>Broad categorization of the contents of the data file.</t>
   </si>
   <si>
+    <t>data_type</t>
+  </si>
+  <si>
+    <t>The data type</t>
+  </si>
+  <si>
     <t>cv</t>
   </si>
   <si>
@@ -362,6 +368,12 @@
   </si>
   <si>
     <t>proteomics_file</t>
+  </si>
+  <si>
+    <t>unaligned_reads_file</t>
+  </si>
+  <si>
+    <t>aligned_reads_file</t>
   </si>
 </sst>
 </file>
@@ -1556,30 +1568,26 @@
       <c r="T23" s="10"/>
     </row>
     <row r="24">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="18" t="s">
         <v>91</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>85</v>
       </c>
       <c r="C24" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D24" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="20" t="s">
         <v>92</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>93</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
-      <c r="I24" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="J24" s="15">
-        <v>100.0</v>
-      </c>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
@@ -1592,26 +1600,30 @@
       <c r="T24" s="10"/>
     </row>
     <row r="25">
-      <c r="A25" s="18" t="s">
-        <v>94</v>
+      <c r="A25" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="20" t="s">
+      <c r="C25" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>95</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
+      <c r="I25" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="J25" s="15">
+        <v>100.0</v>
+      </c>
       <c r="K25" s="10"/>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
@@ -1662,8 +1674,8 @@
       <c r="B27" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C27" s="8" t="b">
-        <v>0</v>
+      <c r="C27" s="19" t="b">
+        <v>1</v>
       </c>
       <c r="D27" s="20" t="s">
         <v>26</v>
@@ -1672,12 +1684,8 @@
         <v>99</v>
       </c>
       <c r="F27" s="7"/>
-      <c r="G27" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="H27" s="21" t="s">
-        <v>46</v>
-      </c>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
@@ -1692,7 +1700,7 @@
       <c r="T27" s="10"/>
     </row>
     <row r="28">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="18" t="s">
         <v>100</v>
       </c>
       <c r="B28" s="7" t="s">
@@ -1701,15 +1709,19 @@
       <c r="C28" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D28" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="E28" s="21" t="s">
-        <v>102</v>
-      </c>
       <c r="F28" s="7"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
+      <c r="G28" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="21" t="s">
+        <v>46</v>
+      </c>
       <c r="I28" s="10"/>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
@@ -1724,20 +1736,20 @@
       <c r="T28" s="10"/>
     </row>
     <row r="29">
-      <c r="A29" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B29" s="17" t="s">
+      <c r="A29" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="C29" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>72</v>
+      <c r="E29" s="21" t="s">
+        <v>104</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="10"/>
@@ -1753,23 +1765,23 @@
       <c r="Q29" s="10"/>
       <c r="R29" s="10"/>
       <c r="S29" s="10"/>
-      <c r="T29" s="17"/>
+      <c r="T29" s="10"/>
     </row>
     <row r="30">
       <c r="A30" s="18" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C30" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="D30" s="20" t="s">
-        <v>74</v>
+      <c r="D30" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="10"/>
@@ -1785,23 +1797,23 @@
       <c r="Q30" s="10"/>
       <c r="R30" s="10"/>
       <c r="S30" s="10"/>
-      <c r="T30" s="10"/>
+      <c r="T30" s="17"/>
     </row>
     <row r="31">
       <c r="A31" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C31" s="19" t="b">
         <v>1</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="10"/>
@@ -1818,26 +1830,22 @@
       <c r="R31" s="10"/>
       <c r="S31" s="10"/>
       <c r="T31" s="10"/>
-      <c r="U31" s="10"/>
-      <c r="V31" s="10"/>
-      <c r="W31" s="10"/>
-      <c r="X31" s="10"/>
     </row>
     <row r="32">
       <c r="A32" s="18" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="C32" s="8" t="b">
-        <v>0</v>
+        <v>105</v>
+      </c>
+      <c r="C32" s="19" t="b">
+        <v>1</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="10"/>
@@ -1861,19 +1869,19 @@
     </row>
     <row r="33">
       <c r="A33" s="18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C33" s="8" t="b">
         <v>0</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="10"/>
@@ -1890,22 +1898,26 @@
       <c r="R33" s="10"/>
       <c r="S33" s="10"/>
       <c r="T33" s="10"/>
+      <c r="U33" s="10"/>
+      <c r="V33" s="10"/>
+      <c r="W33" s="10"/>
+      <c r="X33" s="10"/>
     </row>
     <row r="34">
-      <c r="A34" s="6" t="s">
-        <v>84</v>
+      <c r="A34" s="18" t="s">
+        <v>81</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C34" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>87</v>
+        <v>0</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>83</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="10"/>
@@ -1925,19 +1937,19 @@
     </row>
     <row r="35">
       <c r="A35" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C35" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>90</v>
+      <c r="D35" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>87</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="10"/>
@@ -1957,29 +1969,25 @@
     </row>
     <row r="36">
       <c r="A36" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C36" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>90</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
-      <c r="I36" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="J36" s="15">
-        <v>100.0</v>
-      </c>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
       <c r="K36" s="10"/>
       <c r="L36" s="10"/>
       <c r="M36" s="10"/>
@@ -1993,25 +2001,25 @@
     </row>
     <row r="37">
       <c r="A37" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="C37" s="19" t="b">
+        <v>106</v>
+      </c>
+      <c r="C37" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="D37" s="20" t="s">
-        <v>26</v>
+      <c r="D37" s="10" t="s">
+        <v>86</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="10"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
       <c r="K37" s="10"/>
       <c r="L37" s="10"/>
       <c r="M37" s="10"/>
@@ -2024,26 +2032,30 @@
       <c r="T37" s="10"/>
     </row>
     <row r="38">
-      <c r="A38" s="18" t="s">
-        <v>96</v>
+      <c r="A38" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="B38" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="C38" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E38" s="20" t="s">
-        <v>97</v>
+        <v>106</v>
+      </c>
+      <c r="C38" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>95</v>
       </c>
       <c r="F38" s="7"/>
       <c r="G38" s="10"/>
       <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="10"/>
+      <c r="I38" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="J38" s="15">
+        <v>100.0</v>
+      </c>
       <c r="K38" s="10"/>
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
@@ -2057,27 +2069,23 @@
     </row>
     <row r="39">
       <c r="A39" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="C39" s="8" t="b">
-        <v>0</v>
+        <v>106</v>
+      </c>
+      <c r="C39" s="19" t="b">
+        <v>1</v>
       </c>
       <c r="D39" s="20" t="s">
         <v>26</v>
       </c>
       <c r="E39" s="20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F39" s="7"/>
-      <c r="G39" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="H39" s="21" t="s">
-        <v>46</v>
-      </c>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
       <c r="I39" s="10"/>
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
@@ -2092,20 +2100,20 @@
       <c r="T39" s="10"/>
     </row>
     <row r="40">
-      <c r="A40" s="21" t="s">
-        <v>100</v>
+      <c r="A40" s="18" t="s">
+        <v>98</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="C40" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D40" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="E40" s="21" t="s">
-        <v>102</v>
+        <v>106</v>
+      </c>
+      <c r="C40" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>99</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="10"/>
@@ -2121,27 +2129,31 @@
       <c r="Q40" s="10"/>
       <c r="R40" s="10"/>
       <c r="S40" s="10"/>
-      <c r="T40" s="17"/>
+      <c r="T40" s="10"/>
     </row>
     <row r="41">
       <c r="A41" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B41" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="C41" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D41" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D41" s="20" t="s">
         <v>26</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="F41" s="7"/>
-      <c r="G41" s="10"/>
-      <c r="H41" s="10"/>
+      <c r="G41" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H41" s="21" t="s">
+        <v>46</v>
+      </c>
       <c r="I41" s="10"/>
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
@@ -2153,23 +2165,23 @@
       <c r="Q41" s="10"/>
       <c r="R41" s="10"/>
       <c r="S41" s="10"/>
-      <c r="T41" s="17"/>
+      <c r="T41" s="10"/>
     </row>
     <row r="42">
-      <c r="A42" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="C42" s="19" t="b">
-        <v>1</v>
-      </c>
-      <c r="D42" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="E42" s="20" t="s">
-        <v>75</v>
+      <c r="A42" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C42" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D42" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E42" s="21" t="s">
+        <v>104</v>
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="10"/>
@@ -2185,23 +2197,23 @@
       <c r="Q42" s="10"/>
       <c r="R42" s="10"/>
       <c r="S42" s="10"/>
-      <c r="T42" s="10"/>
+      <c r="T42" s="17"/>
     </row>
     <row r="43">
       <c r="A43" s="18" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C43" s="19" t="b">
         <v>1</v>
       </c>
-      <c r="D43" s="20" t="s">
-        <v>77</v>
+      <c r="D43" s="7" t="s">
+        <v>26</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="10"/>
@@ -2217,23 +2229,23 @@
       <c r="Q43" s="10"/>
       <c r="R43" s="10"/>
       <c r="S43" s="10"/>
-      <c r="T43" s="10"/>
+      <c r="T43" s="17"/>
     </row>
     <row r="44">
       <c r="A44" s="18" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" s="8" t="b">
-        <v>0</v>
+        <v>107</v>
+      </c>
+      <c r="C44" s="19" t="b">
+        <v>1</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="10"/>
@@ -2253,19 +2265,19 @@
     </row>
     <row r="45">
       <c r="A45" s="18" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="C45" s="8" t="b">
-        <v>0</v>
+        <v>107</v>
+      </c>
+      <c r="C45" s="19" t="b">
+        <v>1</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E45" s="20" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="10"/>
@@ -2284,20 +2296,20 @@
       <c r="T45" s="10"/>
     </row>
     <row r="46">
-      <c r="A46" s="6" t="s">
-        <v>84</v>
+      <c r="A46" s="18" t="s">
+        <v>79</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C46" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>87</v>
+        <v>0</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>80</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="10"/>
@@ -2314,26 +2326,22 @@
       <c r="R46" s="10"/>
       <c r="S46" s="10"/>
       <c r="T46" s="10"/>
-      <c r="U46" s="10"/>
-      <c r="V46" s="10"/>
-      <c r="W46" s="10"/>
-      <c r="X46" s="10"/>
     </row>
     <row r="47">
-      <c r="A47" s="6" t="s">
-        <v>88</v>
+      <c r="A47" s="18" t="s">
+        <v>81</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C47" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D47" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="E47" s="10" t="s">
-        <v>90</v>
+        <v>0</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E47" s="20" t="s">
+        <v>83</v>
       </c>
       <c r="F47" s="7"/>
       <c r="G47" s="10"/>
@@ -2350,36 +2358,28 @@
       <c r="R47" s="10"/>
       <c r="S47" s="10"/>
       <c r="T47" s="10"/>
-      <c r="U47" s="10"/>
-      <c r="V47" s="10"/>
-      <c r="W47" s="10"/>
-      <c r="X47" s="10"/>
     </row>
     <row r="48">
       <c r="A48" s="6" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C48" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>92</v>
+        <v>1</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>86</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F48" s="7"/>
       <c r="G48" s="10"/>
       <c r="H48" s="10"/>
-      <c r="I48" s="15">
-        <v>0.0</v>
-      </c>
-      <c r="J48" s="15">
-        <v>100.0</v>
-      </c>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
       <c r="K48" s="10"/>
       <c r="L48" s="10"/>
       <c r="M48" s="10"/>
@@ -2390,22 +2390,26 @@
       <c r="R48" s="10"/>
       <c r="S48" s="10"/>
       <c r="T48" s="10"/>
+      <c r="U48" s="10"/>
+      <c r="V48" s="10"/>
+      <c r="W48" s="10"/>
+      <c r="X48" s="10"/>
     </row>
     <row r="49">
-      <c r="A49" s="18" t="s">
-        <v>94</v>
+      <c r="A49" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="C49" s="19" t="b">
+        <v>108</v>
+      </c>
+      <c r="C49" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="D49" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E49" s="20" t="s">
-        <v>95</v>
+      <c r="D49" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>90</v>
       </c>
       <c r="F49" s="7"/>
       <c r="G49" s="10"/>
@@ -2422,28 +2426,32 @@
       <c r="R49" s="10"/>
       <c r="S49" s="10"/>
       <c r="T49" s="10"/>
+      <c r="U49" s="10"/>
+      <c r="V49" s="10"/>
+      <c r="W49" s="10"/>
+      <c r="X49" s="10"/>
     </row>
     <row r="50">
       <c r="A50" s="18" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="C50" s="19" t="b">
+        <v>108</v>
+      </c>
+      <c r="C50" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="D50" s="20" t="s">
-        <v>26</v>
+      <c r="D50" s="10" t="s">
+        <v>86</v>
       </c>
       <c r="E50" s="20" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="10"/>
       <c r="H50" s="10"/>
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
+      <c r="I50" s="15"/>
+      <c r="J50" s="15"/>
       <c r="K50" s="10"/>
       <c r="L50" s="10"/>
       <c r="M50" s="10"/>
@@ -2456,30 +2464,30 @@
       <c r="T50" s="10"/>
     </row>
     <row r="51">
-      <c r="A51" s="18" t="s">
-        <v>98</v>
+      <c r="A51" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C51" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="D51" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E51" s="20" t="s">
-        <v>99</v>
+      <c r="D51" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>95</v>
       </c>
       <c r="F51" s="7"/>
-      <c r="G51" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="H51" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="I51" s="10"/>
-      <c r="J51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="J51" s="15">
+        <v>100.0</v>
+      </c>
       <c r="K51" s="10"/>
       <c r="L51" s="10"/>
       <c r="M51" s="10"/>
@@ -2492,82 +2500,729 @@
       <c r="T51" s="10"/>
     </row>
     <row r="52">
-      <c r="A52" s="21" t="s">
+      <c r="A52" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D52" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E52" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="F52" s="7"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10"/>
+      <c r="K52" s="10"/>
+      <c r="L52" s="10"/>
+      <c r="M52" s="10"/>
+      <c r="N52" s="10"/>
+      <c r="O52" s="10"/>
+      <c r="P52" s="10"/>
+      <c r="Q52" s="10"/>
+      <c r="R52" s="10"/>
+      <c r="S52" s="10"/>
+      <c r="T52" s="10"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D53" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E53" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="F53" s="7"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10"/>
+      <c r="K53" s="10"/>
+      <c r="L53" s="10"/>
+      <c r="M53" s="10"/>
+      <c r="N53" s="10"/>
+      <c r="O53" s="10"/>
+      <c r="P53" s="10"/>
+      <c r="Q53" s="10"/>
+      <c r="R53" s="10"/>
+      <c r="S53" s="10"/>
+      <c r="T53" s="10"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="B52" s="20" t="s">
-        <v>106</v>
-      </c>
-      <c r="C52" s="8" t="b">
+      <c r="B54" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C54" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="D52" s="21" t="s">
+      <c r="D54" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E54" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="E52" s="21" t="s">
+      <c r="F54" s="7"/>
+      <c r="G54" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H54" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="I54" s="10"/>
+      <c r="J54" s="10"/>
+      <c r="K54" s="10"/>
+      <c r="L54" s="10"/>
+      <c r="M54" s="10"/>
+      <c r="N54" s="10"/>
+      <c r="O54" s="10"/>
+      <c r="P54" s="10"/>
+      <c r="Q54" s="10"/>
+      <c r="R54" s="10"/>
+      <c r="S54" s="10"/>
+      <c r="T54" s="10"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="O52" s="10"/>
-    </row>
-    <row r="53">
-      <c r="O53" s="10"/>
-    </row>
-    <row r="54">
-      <c r="O54" s="10"/>
-    </row>
-    <row r="55">
+      <c r="B55" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="C55" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D55" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E55" s="21" t="s">
+        <v>104</v>
+      </c>
       <c r="O55" s="10"/>
     </row>
     <row r="56">
+      <c r="A56" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B56" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C56" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F56" s="7"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
+      <c r="J56" s="10"/>
+      <c r="K56" s="10"/>
+      <c r="L56" s="10"/>
+      <c r="M56" s="10"/>
+      <c r="N56" s="10"/>
       <c r="O56" s="10"/>
+      <c r="P56" s="10"/>
+      <c r="Q56" s="10"/>
+      <c r="R56" s="10"/>
+      <c r="S56" s="10"/>
+      <c r="T56" s="10"/>
+      <c r="U56" s="10"/>
+      <c r="V56" s="10"/>
+      <c r="W56" s="10"/>
+      <c r="X56" s="10"/>
     </row>
     <row r="57">
+      <c r="A57" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C57" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F57" s="7"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="10"/>
+      <c r="K57" s="10"/>
+      <c r="L57" s="10"/>
+      <c r="M57" s="10"/>
+      <c r="N57" s="10"/>
       <c r="O57" s="10"/>
+      <c r="P57" s="10"/>
+      <c r="Q57" s="10"/>
+      <c r="R57" s="10"/>
+      <c r="S57" s="10"/>
+      <c r="T57" s="10"/>
+      <c r="U57" s="10"/>
+      <c r="V57" s="10"/>
+      <c r="W57" s="10"/>
+      <c r="X57" s="10"/>
     </row>
     <row r="58">
+      <c r="A58" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C58" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="F58" s="7"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="15"/>
+      <c r="K58" s="10"/>
+      <c r="L58" s="10"/>
+      <c r="M58" s="10"/>
+      <c r="N58" s="10"/>
       <c r="O58" s="10"/>
+      <c r="P58" s="10"/>
+      <c r="Q58" s="10"/>
+      <c r="R58" s="10"/>
+      <c r="S58" s="10"/>
+      <c r="T58" s="10"/>
     </row>
     <row r="59">
+      <c r="A59" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B59" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C59" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F59" s="7"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="J59" s="15">
+        <v>100.0</v>
+      </c>
+      <c r="K59" s="10"/>
+      <c r="L59" s="10"/>
+      <c r="M59" s="10"/>
+      <c r="N59" s="10"/>
       <c r="O59" s="10"/>
+      <c r="P59" s="10"/>
+      <c r="Q59" s="10"/>
+      <c r="R59" s="10"/>
+      <c r="S59" s="10"/>
+      <c r="T59" s="10"/>
     </row>
     <row r="60">
+      <c r="A60" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B60" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="F60" s="7"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="10"/>
+      <c r="J60" s="10"/>
+      <c r="K60" s="10"/>
+      <c r="L60" s="10"/>
+      <c r="M60" s="10"/>
+      <c r="N60" s="10"/>
       <c r="O60" s="10"/>
+      <c r="P60" s="10"/>
+      <c r="Q60" s="10"/>
+      <c r="R60" s="10"/>
+      <c r="S60" s="10"/>
+      <c r="T60" s="10"/>
     </row>
     <row r="61">
+      <c r="A61" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C61" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E61" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="F61" s="7"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="10"/>
+      <c r="I61" s="10"/>
+      <c r="J61" s="10"/>
+      <c r="K61" s="10"/>
+      <c r="L61" s="10"/>
+      <c r="M61" s="10"/>
+      <c r="N61" s="10"/>
       <c r="O61" s="10"/>
+      <c r="P61" s="10"/>
+      <c r="Q61" s="10"/>
+      <c r="R61" s="10"/>
+      <c r="S61" s="10"/>
+      <c r="T61" s="10"/>
     </row>
     <row r="62">
+      <c r="A62" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C62" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D62" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E62" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="F62" s="7"/>
+      <c r="G62" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H62" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="I62" s="10"/>
+      <c r="J62" s="10"/>
+      <c r="K62" s="10"/>
+      <c r="L62" s="10"/>
+      <c r="M62" s="10"/>
+      <c r="N62" s="10"/>
       <c r="O62" s="10"/>
+      <c r="P62" s="10"/>
+      <c r="Q62" s="10"/>
+      <c r="R62" s="10"/>
+      <c r="S62" s="10"/>
+      <c r="T62" s="10"/>
     </row>
     <row r="63">
+      <c r="A63" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C63" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D63" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E63" s="21" t="s">
+        <v>104</v>
+      </c>
       <c r="O63" s="10"/>
     </row>
     <row r="64">
+      <c r="A64" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B64" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C64" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F64" s="7"/>
+      <c r="G64" s="10"/>
+      <c r="H64" s="10"/>
+      <c r="I64" s="10"/>
+      <c r="J64" s="10"/>
+      <c r="K64" s="10"/>
+      <c r="L64" s="10"/>
+      <c r="M64" s="10"/>
+      <c r="N64" s="10"/>
       <c r="O64" s="10"/>
+      <c r="P64" s="10"/>
+      <c r="Q64" s="10"/>
+      <c r="R64" s="10"/>
+      <c r="S64" s="10"/>
+      <c r="T64" s="10"/>
+      <c r="U64" s="10"/>
+      <c r="V64" s="10"/>
+      <c r="W64" s="10"/>
+      <c r="X64" s="10"/>
+      <c r="Y64" s="10"/>
+      <c r="Z64" s="10"/>
+      <c r="AA64" s="10"/>
     </row>
     <row r="65">
+      <c r="A65" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C65" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F65" s="7"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
+      <c r="I65" s="10"/>
+      <c r="J65" s="10"/>
+      <c r="K65" s="10"/>
+      <c r="L65" s="10"/>
+      <c r="M65" s="10"/>
+      <c r="N65" s="10"/>
       <c r="O65" s="10"/>
+      <c r="P65" s="10"/>
+      <c r="Q65" s="10"/>
+      <c r="R65" s="10"/>
+      <c r="S65" s="10"/>
+      <c r="T65" s="10"/>
+      <c r="U65" s="10"/>
+      <c r="V65" s="10"/>
+      <c r="W65" s="10"/>
+      <c r="X65" s="10"/>
+      <c r="Y65" s="10"/>
+      <c r="Z65" s="10"/>
+      <c r="AA65" s="10"/>
     </row>
     <row r="66">
+      <c r="A66" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C66" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F66" s="7"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="10"/>
+      <c r="K66" s="10"/>
+      <c r="L66" s="10"/>
+      <c r="M66" s="10"/>
+      <c r="N66" s="10"/>
       <c r="O66" s="10"/>
+      <c r="P66" s="10"/>
+      <c r="Q66" s="10"/>
+      <c r="R66" s="10"/>
+      <c r="S66" s="10"/>
+      <c r="T66" s="10"/>
+      <c r="U66" s="10"/>
+      <c r="V66" s="10"/>
+      <c r="W66" s="10"/>
+      <c r="X66" s="10"/>
+      <c r="Y66" s="10"/>
+      <c r="Z66" s="10"/>
+      <c r="AA66" s="10"/>
     </row>
     <row r="67">
+      <c r="A67" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C67" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F67" s="7"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="15">
+        <v>0.0</v>
+      </c>
+      <c r="J67" s="15">
+        <v>100.0</v>
+      </c>
+      <c r="K67" s="10"/>
+      <c r="L67" s="10"/>
+      <c r="M67" s="10"/>
+      <c r="N67" s="10"/>
       <c r="O67" s="10"/>
+      <c r="P67" s="10"/>
+      <c r="Q67" s="10"/>
+      <c r="R67" s="10"/>
+      <c r="S67" s="10"/>
+      <c r="T67" s="10"/>
+      <c r="U67" s="10"/>
+      <c r="V67" s="10"/>
+      <c r="W67" s="10"/>
+      <c r="X67" s="10"/>
+      <c r="Y67" s="10"/>
+      <c r="Z67" s="10"/>
+      <c r="AA67" s="10"/>
     </row>
     <row r="68">
+      <c r="A68" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C68" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E68" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F68" s="7"/>
+      <c r="G68" s="10"/>
+      <c r="H68" s="10"/>
+      <c r="I68" s="10"/>
+      <c r="J68" s="10"/>
+      <c r="K68" s="10"/>
+      <c r="L68" s="10"/>
+      <c r="M68" s="10"/>
+      <c r="N68" s="10"/>
       <c r="O68" s="10"/>
+      <c r="P68" s="10"/>
+      <c r="Q68" s="10"/>
+      <c r="R68" s="10"/>
+      <c r="S68" s="10"/>
+      <c r="T68" s="10"/>
+      <c r="U68" s="10"/>
+      <c r="V68" s="10"/>
+      <c r="W68" s="10"/>
+      <c r="X68" s="10"/>
+      <c r="Y68" s="10"/>
+      <c r="Z68" s="10"/>
+      <c r="AA68" s="10"/>
     </row>
     <row r="69">
+      <c r="A69" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B69" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C69" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F69" s="7"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+      <c r="I69" s="10"/>
+      <c r="J69" s="10"/>
+      <c r="K69" s="10"/>
+      <c r="L69" s="10"/>
+      <c r="M69" s="10"/>
+      <c r="N69" s="10"/>
       <c r="O69" s="10"/>
+      <c r="P69" s="10"/>
+      <c r="Q69" s="10"/>
+      <c r="R69" s="10"/>
+      <c r="S69" s="10"/>
+      <c r="T69" s="10"/>
+      <c r="U69" s="10"/>
+      <c r="V69" s="10"/>
+      <c r="W69" s="10"/>
+      <c r="X69" s="10"/>
+      <c r="Y69" s="10"/>
+      <c r="Z69" s="10"/>
+      <c r="AA69" s="10"/>
     </row>
     <row r="70">
+      <c r="A70" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B70" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C70" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F70" s="7"/>
+      <c r="G70" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H70" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I70" s="10"/>
+      <c r="J70" s="10"/>
+      <c r="K70" s="10"/>
+      <c r="L70" s="10"/>
+      <c r="M70" s="10"/>
+      <c r="N70" s="10"/>
       <c r="O70" s="10"/>
+      <c r="P70" s="10"/>
+      <c r="Q70" s="10"/>
+      <c r="R70" s="10"/>
+      <c r="S70" s="10"/>
+      <c r="T70" s="10"/>
+      <c r="U70" s="10"/>
+      <c r="V70" s="10"/>
+      <c r="W70" s="10"/>
+      <c r="X70" s="10"/>
+      <c r="Y70" s="10"/>
+      <c r="Z70" s="10"/>
+      <c r="AA70" s="10"/>
     </row>
     <row r="71">
+      <c r="A71" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B71" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C71" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F71" s="10"/>
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
+      <c r="I71" s="10"/>
+      <c r="J71" s="10"/>
+      <c r="K71" s="10"/>
+      <c r="L71" s="10"/>
+      <c r="M71" s="10"/>
+      <c r="N71" s="10"/>
       <c r="O71" s="10"/>
+      <c r="P71" s="10"/>
+      <c r="Q71" s="10"/>
+      <c r="R71" s="10"/>
+      <c r="S71" s="10"/>
+      <c r="T71" s="10"/>
+      <c r="U71" s="10"/>
+      <c r="V71" s="10"/>
+      <c r="W71" s="10"/>
+      <c r="X71" s="10"/>
+      <c r="Y71" s="10"/>
+      <c r="Z71" s="10"/>
+      <c r="AA71" s="10"/>
     </row>
     <row r="72">
+      <c r="A72" s="10"/>
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="10"/>
+      <c r="G72" s="10"/>
+      <c r="H72" s="10"/>
+      <c r="I72" s="10"/>
+      <c r="J72" s="10"/>
+      <c r="K72" s="10"/>
+      <c r="L72" s="10"/>
+      <c r="M72" s="10"/>
+      <c r="N72" s="10"/>
       <c r="O72" s="10"/>
+      <c r="P72" s="10"/>
+      <c r="Q72" s="10"/>
+      <c r="R72" s="10"/>
+      <c r="S72" s="10"/>
+      <c r="T72" s="10"/>
+      <c r="U72" s="10"/>
+      <c r="V72" s="10"/>
+      <c r="W72" s="10"/>
+      <c r="X72" s="10"/>
+      <c r="Y72" s="10"/>
+      <c r="Z72" s="10"/>
+      <c r="AA72" s="10"/>
     </row>
     <row r="73">
       <c r="O73" s="10"/>
@@ -5359,48 +6014,36 @@
     <row r="1002">
       <c r="O1002" s="10"/>
     </row>
+    <row r="1003">
+      <c r="O1003" s="10"/>
+    </row>
+    <row r="1004">
+      <c r="O1004" s="10"/>
+    </row>
+    <row r="1005">
+      <c r="O1005" s="10"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$T$1002">
-    <sortState ref="A1:T1002">
-      <sortCondition ref="D1:D1002"/>
-      <sortCondition ref="B1:B1002"/>
+  <autoFilter ref="$A$1:$T$1005">
+    <sortState ref="A1:T1005">
+      <sortCondition ref="D1:D1005"/>
+      <sortCondition ref="B1:B1005"/>
     </sortState>
   </autoFilter>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="B2:B28 B41:B45">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D8:D9">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B46:B52">
-      <formula1>#REF!</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="D5">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="D4">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D23">
+    <dataValidation type="list" allowBlank="1" sqref="D22 D24 D37 D50 D58 D66">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D13 D20:D21 D32:D33 D44:D45">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D22 D27 D34 D39 D46 D51">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G2:G51">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D18:D19 D30:D31 D42:D43">
+    <dataValidation type="list" allowBlank="1" sqref="G2:G54 G56:G62 G64:G70">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="D10">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D17 D25:D26 D29 D37:D38 D41 D49:D50">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="D2:D3">
@@ -5409,20 +6052,62 @@
     <dataValidation type="list" allowBlank="1" sqref="D6:D7">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D24 D36 D48">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D11:D12">
-      <formula1>#REF!</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="D14:D16">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D35 D47">
+    <dataValidation type="list" allowBlank="1" sqref="B35:B42 B56:B71">
+      <formula1>"sample,subject,medical_history,demographic,lipidomics_file,core_metadata_collections"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D49 D57 D65">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B34:B40">
-      <formula1>"sample,subject,medical_history,demographic,lipidomics_file,core_metadata_collections"</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="B2:B29 B43:B47">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D8:D9">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="B48:B55">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D23">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D13 D20:D21 D31:D32 D39:D40 D43">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D18:D19 D26:D27 D30">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D28 D35">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D33:D34 D44:D45 D52:D53 D60:D61 D68:D69">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D17">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D41 D48 D56 D64">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D46:D47">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D38">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D11:D12 D25">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D51 D59 D67">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D54 D62 D70">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D36">
+      <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>

</xml_diff>